<commit_message>
Remove staff name from allocation template
</commit_message>
<xml_diff>
--- a/storage/app/templates/allocation_template.xlsx
+++ b/storage/app/templates/allocation_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenn\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\gifms-core\storage\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0710EC93-3CAE-4961-8CFF-3BD1FCDFD7FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8205"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,19 +42,19 @@
     <t>CHKENYDINOH1</t>
   </si>
   <si>
-    <t>RAMADHAN WANGATIA  Reimbursement, airtime - Cell usage, 2018 April</t>
-  </si>
-  <si>
     <t>CHKENYCEM4</t>
   </si>
   <si>
     <t>CHKENYHLSTP3</t>
+  </si>
+  <si>
+    <t>Reimbursement, airtime - Cell usage, 2018 April</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -375,22 +376,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.53515625" customWidth="1"/>
+    <col min="5" max="5" width="17.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -405,7 +406,7 @@
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -413,44 +414,44 @@
         <v>66100</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2">
         <v>462.24</v>
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2">
         <v>66100</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2">
         <v>513.6</v>
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
         <v>66100</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2">
         <v>410.88</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>

</xml_diff>